<commit_message>
Added support for local execution videos
</commit_message>
<xml_diff>
--- a/src/test/resources/TestingFile.xlsx
+++ b/src/test/resources/TestingFile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>url</t>
   </si>
@@ -496,7 +496,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -539,7 +539,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>30</v>
@@ -564,7 +564,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -617,10 +617,10 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>109</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -629,7 +629,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
         <v>26</v>
@@ -651,8 +651,8 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>20</v>
+      <c r="D3" s="4">
+        <v>109</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -683,8 +683,8 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>20</v>
+      <c r="D4" s="4">
+        <v>109</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -715,14 +715,14 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
+      <c r="D5" s="4">
+        <v>109</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
       </c>
       <c r="F5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Updated video recording code to add proper synchronization
</commit_message>
<xml_diff>
--- a/src/test/resources/TestingFile.xlsx
+++ b/src/test/resources/TestingFile.xlsx
@@ -539,7 +539,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>30</v>
@@ -564,7 +564,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -722,10 +722,10 @@
         <v>25</v>
       </c>
       <c r="F5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Added code to take dynamic screenshots
</commit_message>
<xml_diff>
--- a/src/test/resources/TestingFile.xlsx
+++ b/src/test/resources/TestingFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Count" sheetId="3" r:id="rId1"/>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -525,7 +525,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>19</v>
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -626,10 +626,10 @@
         <v>25</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
         <v>26</v>
@@ -725,7 +725,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>20</v>

</xml_diff>